<commit_message>
Updated new-domain rule for the hack to fix MoM defect: removed Panama locales and added Haredi Hebrew
</commit_message>
<xml_diff>
--- a/config_new.xlsx
+++ b/config_new.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="485">
   <si>
     <t xml:space="preserve">search</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t xml:space="preserve">2024.11.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updated on 2024.12.17 with exception to not run on segment 66b48cbf98f469.15102915_80b6c808128cc0e7f1953f70140d5f72_5 </t>
   </si>
   <si>
     <t xml:space="preserve">(&lt;div&gt;\s+&lt;strong&gt;)((?:Key:?)\s*)(&lt;/strong&gt;\s+&lt;/div&gt;)</t>
@@ -1464,7 +1467,7 @@
     <t xml:space="preserve">### MoM defects ### </t>
   </si>
   <si>
-    <t xml:space="preserve">(&lt;label key="ST003_38b463f7d6223477fd819aaa8473dc35_2" its:localeFilterList="fr-ZZ,zh-Hant-ZZ,es-DO,fr-FR,es-GT,ja-JP,en-KE,sq-XK,sr-XK,ky-KG,ru-KG,uz-KG,ms-MY,en-MY,mk-MK,sq-MK,es-PA,en-PA,en-PH,pt-PT,vi-VN,sq-AL,en-AE,ar-AE,es-AR,hy-AM,en-AU,bg-BG,pt-BR,en-BN,ms-BN,en-CA,fr-CA,de-CH,fr-CH,it-CH,es-CL,es-CO,es-CR,cs-CZ,da-DK,fo-DK,es-EC,ar-EG,en-EG,eu-ES,ca-ES,gl-ES,es-ES,ca-ES-valencia,et-EE,ru-EE,fi-FI,sv-FI,ka-GE,az-GE,ru-GE,el-GR,zh-HK,en-HK,hr-HR,hu-HU,id-ID,en-IE,ga-IE,ar-IL,he-IL,ar-JO,kk-KZ,ru-KZ,ko-KR,en-LB,fr-LB,lt-LT,pl-LT,ru-LT,lv-LV,en-MO,pt-MO,zh-MO,ar-MA,fr-MA,ro-MD,ru-MD,es-MX,en-MT,mt-MT,cnr-ME,sq-ME,mn-MN,kk-MN,en-NZ,es-PE,pl-PL,es-PY,ar-PS,en-PS,ar-QA,en-QA,az-QZ,ru-QZ,el-CY,en-CY,en-GB-scotland,en-GB-x-excscotl,cy-GB,ro-RO,hu-RO,ar-SA,en-SA,en-SG,es-SV,sr-RS,hu-RS,sl-SI,sl-SI-x-isced2,zh-TW,th-TH,tr-TR,uk-UA,es-UY,en-US,uz-UZ,ru-UZ,kaa-UZ,zh-CN,is-IS,zh-XX,ru-XX,en-XX,ar-YY)(" its:localeFilterType="include"&gt;)</t>
+    <t xml:space="preserve">(&lt;label key="ST003_38b463f7d6223477fd819aaa8473dc35_2" its:localeFilterList="fr-ZZ,zh-Hant-ZZ,es-DO,fr-FR,es-GT,ja-JP,en-KE,sq-XK,sr-XK,ky-KG,ru-KG,uz-KG,ms-MY,en-MY,mk-MK,sq-MK,en-PH,pt-PT,vi-VN,sq-AL,en-AE,ar-AE,es-AR,hy-AM,en-AU,bg-BG,pt-BR,en-BN,ms-BN,en-CA,fr-CA,de-CH,fr-CH,it-CH,es-CL,es-CO,es-CR,cs-CZ,da-DK,fo-DK,es-EC,ar-EG,en-EG,eu-ES,ca-ES,gl-ES,es-ES,ca-ES-valencia,et-EE,ru-EE,fi-FI,sv-FI,ka-GE,az-GE,ru-GE,el-GR,zh-HK,en-HK,hr-HR,hu-HU,id-ID,en-IE,ga-IE,ar-IL,he-IL,he-IL-x-haredi,ar-JO,kk-KZ,ru-KZ,ko-KR,en-LB,fr-LB,lt-LT,pl-LT,ru-LT,lv-LV,en-MO,pt-MO,zh-MO,ar-MA,fr-MA,ro-MD,ru-MD,es-MX,en-MT,mt-MT,cnr-ME,sq-ME,mn-MN,kk-MN,en-NZ,es-PE,pl-PL,es-PY,ar-PS,en-PS,ar-QA,en-QA,az-QZ,ru-QZ,el-CY,en-CY,en-GB-scotland,en-GB-x-excscotl,cy-GB,ro-RO,hu-RO,ar-SA,en-SA,en-SG,es-SV,sr-RS,hu-RS,sl-SI,sl-SI-x-isced2,zh-TW,th-TH,tr-TR,uk-UA,es-UY,en-US,uz-UZ,ru-UZ,kaa-UZ,zh-CN,is-IS,zh-XX,ru-XX,en-XX,ar-YY)(" its:localeFilterType="include"&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">$1,de-AT,fr-BE,nl-BE,de-BE,de-DE,it-IT,de-IT,de-LU,fr-LU,en-LU,nl-NL,nb-NO,nn-NO,sk-SK,hu-SK,en-SE,sv-SE,de-XX$2</t>
@@ -1815,32 +1818,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;em&gt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">\u200C]?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(&amp;lt;Ethnic/national minorities or indigenous communities&amp;gt;)’</t>
-    </r>
+    <t xml:space="preserve">&lt;em&gt;[\u200C]?(&amp;lt;Ethnic/national minorities or indigenous communities&amp;gt;)’</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;em&gt;‌‘$1’</t>
@@ -2039,6 +2017,21 @@
   <si>
     <t xml:space="preserve">&amp;lt;When I listen songs in English I can understand their meaning&amp;gt;</t>
   </si>
+  <si>
+    <t xml:space="preserve">reverted in 2024-12-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row 108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(?&lt;!to bring groundwater to the surface for their water supply)&lt;/span&gt;[\s\n]+&lt;span&gt;(\.\s*)&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restored on 2024-12-18 (this is the version that would restore the segmentation defect, this was live for one day, but then both entries were added to all Tms)</t>
+  </si>
 </sst>
 </file>
 
@@ -2048,7 +2041,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2189,11 +2182,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2480,7 +2468,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2594,14 +2582,14 @@
   <dimension ref="A1:AN1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="A243" activeCellId="0" sqref="A243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="173.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="110.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="90.81"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="2" width="9.13"/>
@@ -2911,152 +2899,155 @@
       <c r="F20" s="12" t="s">
         <v>45</v>
       </c>
+      <c r="G20" s="12" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="24" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
@@ -3066,11 +3057,11 @@
     </row>
     <row r="39" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
@@ -3082,13 +3073,13 @@
     </row>
     <row r="40" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -3100,10 +3091,10 @@
     </row>
     <row r="41" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -3116,370 +3107,370 @@
     </row>
     <row r="42" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="68" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="14" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="72" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="73" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="75" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="76" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="77" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="79" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="80" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="81" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B83" s="14" t="s">
         <v>130</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="84" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="86" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B86" s="16" t="s">
         <v>134</v>
-      </c>
-      <c r="B86" s="16" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="87" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C87" s="13"/>
       <c r="D87" s="13"/>
@@ -3492,10 +3483,10 @@
     </row>
     <row r="88" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C88" s="13"/>
       <c r="D88" s="13"/>
@@ -3508,10 +3499,10 @@
     </row>
     <row r="89" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
@@ -3524,10 +3515,10 @@
     </row>
     <row r="90" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
@@ -3540,13 +3531,13 @@
     </row>
     <row r="91" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
@@ -3558,10 +3549,10 @@
     </row>
     <row r="92" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
@@ -3574,10 +3565,10 @@
     </row>
     <row r="93" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
@@ -3590,10 +3581,10 @@
     </row>
     <row r="94" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
@@ -3606,10 +3597,10 @@
     </row>
     <row r="95" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
@@ -3622,14 +3613,14 @@
     </row>
     <row r="96" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B96" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="8"/>
@@ -3640,14 +3631,14 @@
     </row>
     <row r="97" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B97" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E97" s="8"/>
       <c r="F97" s="8"/>
@@ -3656,14 +3647,14 @@
     </row>
     <row r="98" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="8"/>
@@ -3672,97 +3663,97 @@
     </row>
     <row r="99" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="18" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C99" s="18"/>
       <c r="D99" s="19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="100" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B100" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C100" s="18"/>
       <c r="D100" s="19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="101" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C101" s="18"/>
     </row>
     <row r="102" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C102" s="18"/>
     </row>
     <row r="103" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B103" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C103" s="18"/>
     </row>
     <row r="104" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C104" s="18"/>
     </row>
     <row r="105" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C105" s="18"/>
     </row>
     <row r="106" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C106" s="18"/>
     </row>
     <row r="107" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B107" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C107" s="18"/>
     </row>
     <row r="108" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C108" s="18"/>
       <c r="D108" s="19"/>
@@ -3773,10 +3764,10 @@
     </row>
     <row r="109" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C109" s="12"/>
       <c r="D109" s="8"/>
@@ -3789,10 +3780,10 @@
     </row>
     <row r="110" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C110" s="12"/>
       <c r="D110" s="8"/>
@@ -3805,10 +3796,10 @@
     </row>
     <row r="111" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
@@ -3821,10 +3812,10 @@
     </row>
     <row r="112" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
@@ -3837,10 +3828,10 @@
     </row>
     <row r="113" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
@@ -3853,10 +3844,10 @@
     </row>
     <row r="114" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
@@ -3869,10 +3860,10 @@
     </row>
     <row r="115" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C115" s="24"/>
       <c r="D115" s="24"/>
@@ -3885,10 +3876,10 @@
     </row>
     <row r="116" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="23" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C116" s="24"/>
       <c r="D116" s="24"/>
@@ -3901,10 +3892,10 @@
     </row>
     <row r="117" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="23" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C117" s="24"/>
       <c r="D117" s="24"/>
@@ -3917,10 +3908,10 @@
     </row>
     <row r="118" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="23" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B118" s="23" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C118" s="24"/>
       <c r="D118" s="24"/>
@@ -3933,10 +3924,10 @@
     </row>
     <row r="119" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="16" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
@@ -3949,10 +3940,10 @@
     </row>
     <row r="120" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
@@ -3965,10 +3956,10 @@
     </row>
     <row r="121" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="16" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
@@ -3981,10 +3972,10 @@
     </row>
     <row r="122" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
@@ -3997,10 +3988,10 @@
     </row>
     <row r="123" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="16" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
@@ -4013,10 +4004,10 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="16" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
@@ -4030,11 +4021,11 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B125" s="12"/>
       <c r="C125" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D125" s="8"/>
       <c r="E125" s="8"/>
@@ -4047,10 +4038,10 @@
     </row>
     <row r="126" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D126" s="8"/>
       <c r="E126" s="8"/>
@@ -4062,13 +4053,13 @@
     </row>
     <row r="127" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D127" s="8"/>
       <c r="E127" s="8"/>
@@ -4080,10 +4071,10 @@
     </row>
     <row r="128" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D128" s="8"/>
       <c r="E128" s="8"/>
@@ -4095,10 +4086,10 @@
     </row>
     <row r="129" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C129" s="12"/>
       <c r="D129" s="8"/>
@@ -4111,10 +4102,10 @@
     </row>
     <row r="130" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C130" s="12"/>
       <c r="D130" s="8"/>
@@ -4127,10 +4118,10 @@
     </row>
     <row r="131" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C131" s="14"/>
       <c r="D131" s="24"/>
@@ -4143,10 +4134,10 @@
     </row>
     <row r="132" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C132" s="14"/>
       <c r="D132" s="24"/>
@@ -4159,14 +4150,14 @@
     </row>
     <row r="133" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C133" s="8"/>
       <c r="D133" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E133" s="8"/>
       <c r="F133" s="8"/>
@@ -4175,10 +4166,10 @@
     </row>
     <row r="134" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
@@ -4189,14 +4180,14 @@
     </row>
     <row r="135" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E135" s="8"/>
       <c r="F135" s="8"/>
@@ -4205,37 +4196,37 @@
     </row>
     <row r="136" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="25" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D136" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="137" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="B137" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="D137" s="25" t="s">
         <v>222</v>
-      </c>
-      <c r="B137" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="D137" s="25" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="138" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
@@ -4275,15 +4266,15 @@
     </row>
     <row r="139" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
@@ -4323,10 +4314,10 @@
     </row>
     <row r="140" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
@@ -4371,28 +4362,28 @@
     </row>
     <row r="141" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="142" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="143" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="144" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B144" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C144" s="19"/>
       <c r="D144" s="19"/>
@@ -4406,10 +4397,10 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B145" s="17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C145" s="18"/>
       <c r="D145" s="19"/>
@@ -4423,10 +4414,10 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>233</v>
       </c>
       <c r="D146" s="12"/>
       <c r="E146" s="12"/>
@@ -4439,13 +4430,13 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C147" s="26" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
@@ -4458,13 +4449,13 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D148" s="8"/>
       <c r="E148" s="8"/>
@@ -4477,13 +4468,13 @@
     </row>
     <row r="149" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D149" s="8"/>
       <c r="E149" s="8"/>
@@ -4495,13 +4486,13 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D150" s="8"/>
       <c r="E150" s="8"/>
@@ -4514,13 +4505,13 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C151" s="12" t="s">
         <v>245</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C151" s="12" t="s">
-        <v>244</v>
       </c>
       <c r="D151" s="12"/>
       <c r="E151" s="12"/>
@@ -4533,10 +4524,10 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D152" s="8"/>
       <c r="E152" s="8"/>
@@ -4549,10 +4540,10 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D153" s="8"/>
       <c r="E153" s="8"/>
@@ -4565,13 +4556,13 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D154" s="8"/>
       <c r="E154" s="8"/>
@@ -4584,10 +4575,10 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D155" s="8"/>
       <c r="E155" s="8"/>
@@ -4600,10 +4591,10 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D156" s="8"/>
       <c r="E156" s="8"/>
@@ -4616,10 +4607,10 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D157" s="8"/>
       <c r="E157" s="8"/>
@@ -4632,13 +4623,13 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B158" s="12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D158" s="8"/>
       <c r="E158" s="8"/>
@@ -4651,10 +4642,10 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B159" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D159" s="8"/>
       <c r="E159" s="8"/>
@@ -4667,10 +4658,10 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D160" s="8"/>
       <c r="E160" s="8"/>
@@ -4683,10 +4674,10 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="12" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B161" s="12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D161" s="8"/>
       <c r="E161" s="8"/>
@@ -4699,10 +4690,10 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="12" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B162" s="12" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D162" s="8"/>
       <c r="E162" s="8"/>
@@ -4715,10 +4706,10 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B163" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D163" s="8"/>
       <c r="E163" s="8"/>
@@ -4731,13 +4722,13 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="12" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B164" s="12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D164" s="8"/>
       <c r="E164" s="8"/>
@@ -4750,10 +4741,10 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B165" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D165" s="8"/>
       <c r="E165" s="8"/>
@@ -4766,10 +4757,10 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="12" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B166" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D166" s="8"/>
       <c r="E166" s="8"/>
@@ -4782,10 +4773,10 @@
     </row>
     <row r="167" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="12" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B167" s="12" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C167" s="1"/>
       <c r="D167" s="8"/>
@@ -4796,16 +4787,16 @@
     </row>
     <row r="168" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="12" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B168" s="12" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E168" s="8"/>
       <c r="F168" s="8"/>
@@ -4814,99 +4805,99 @@
     </row>
     <row r="169" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="27" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B169" s="27" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C169" s="28"/>
     </row>
     <row r="170" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="27" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B170" s="27" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C170" s="28" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="171" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="27" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B171" s="27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C171" s="28"/>
     </row>
     <row r="172" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="27" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B172" s="27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C172" s="28"/>
     </row>
     <row r="173" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="27" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B173" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C173" s="28"/>
     </row>
     <row r="174" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="27" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B174" s="27" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C174" s="28"/>
     </row>
     <row r="175" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="27" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B175" s="27" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C175" s="28"/>
     </row>
     <row r="176" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="27" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B176" s="27" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C176" s="28"/>
     </row>
     <row r="177" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="27" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B177" s="27" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C177" s="28"/>
     </row>
     <row r="178" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C178" s="26"/>
     </row>
     <row r="179" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="27" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B179" s="27" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C179" s="28"/>
       <c r="D179" s="27"/>
@@ -4920,10 +4911,10 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="27" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B180" s="27" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C180" s="28"/>
       <c r="D180" s="27"/>
@@ -4937,10 +4928,10 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C181" s="26"/>
       <c r="D181" s="13"/>
@@ -4954,10 +4945,10 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="12" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B182" s="12" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D182" s="8"/>
       <c r="E182" s="8"/>
@@ -4970,10 +4961,10 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="12" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B183" s="12" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D183" s="8"/>
       <c r="E183" s="8"/>
@@ -4986,10 +4977,10 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="12" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B184" s="12" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D184" s="8"/>
       <c r="E184" s="8"/>
@@ -5002,10 +4993,10 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D185" s="8"/>
       <c r="E185" s="8"/>
@@ -5018,10 +5009,10 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D186" s="8"/>
       <c r="E186" s="8"/>
@@ -5034,7 +5025,7 @@
     </row>
     <row r="187" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C187" s="26"/>
       <c r="D187" s="13"/>
@@ -5048,10 +5039,10 @@
     </row>
     <row r="188" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>25</v>
@@ -5067,10 +5058,10 @@
     </row>
     <row r="189" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C189" s="1"/>
       <c r="D189" s="8"/>
@@ -5084,10 +5075,10 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>25</v>
@@ -5103,10 +5094,10 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C191" s="26" t="s">
         <v>25</v>
@@ -5122,10 +5113,10 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C192" s="12" t="s">
         <v>25</v>
@@ -5141,10 +5132,10 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="12" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C193" s="12" t="s">
         <v>25</v>
@@ -5160,13 +5151,13 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B194" s="12" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D194" s="12"/>
       <c r="E194" s="12"/>
@@ -5179,10 +5170,10 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="12" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B195" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C195" s="12" t="s">
         <v>25</v>
@@ -5198,10 +5189,10 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D196" s="8"/>
       <c r="E196" s="8"/>
@@ -5214,19 +5205,19 @@
     </row>
     <row r="197" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C197" s="1"/>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D198" s="8"/>
       <c r="E198" s="8"/>
@@ -5239,10 +5230,10 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="8"/>
@@ -5256,10 +5247,10 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D200" s="8"/>
       <c r="E200" s="8"/>
@@ -5272,10 +5263,10 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D201" s="8"/>
       <c r="E201" s="8"/>
@@ -5288,10 +5279,10 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="29" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D202" s="8"/>
       <c r="E202" s="8"/>
@@ -5304,13 +5295,13 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D203" s="8"/>
       <c r="E203" s="8"/>
@@ -5323,10 +5314,10 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D204" s="8"/>
       <c r="E204" s="8"/>
@@ -5339,10 +5330,10 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D205" s="8"/>
       <c r="E205" s="8"/>
@@ -5355,10 +5346,10 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D206" s="8"/>
       <c r="E206" s="8"/>
@@ -5371,10 +5362,10 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D207" s="8"/>
       <c r="E207" s="8"/>
@@ -5387,10 +5378,10 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D208" s="8"/>
       <c r="E208" s="8"/>
@@ -5403,10 +5394,10 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D209" s="8"/>
       <c r="E209" s="8"/>
@@ -5419,10 +5410,10 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D210" s="8"/>
       <c r="E210" s="8"/>
@@ -5435,10 +5426,10 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D211" s="8"/>
       <c r="E211" s="8"/>
@@ -5451,10 +5442,10 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D212" s="8"/>
       <c r="E212" s="8"/>
@@ -5467,10 +5458,10 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D213" s="8"/>
       <c r="E213" s="8"/>
@@ -5483,10 +5474,10 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D214" s="8"/>
       <c r="E214" s="8"/>
@@ -5499,10 +5490,10 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D215" s="8"/>
       <c r="E215" s="8"/>
@@ -5515,10 +5506,10 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D216" s="8"/>
       <c r="E216" s="8"/>
@@ -5531,10 +5522,10 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D217" s="8"/>
       <c r="E217" s="8"/>
@@ -5547,10 +5538,10 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D218" s="8"/>
       <c r="E218" s="8"/>
@@ -5563,10 +5554,10 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D219" s="8"/>
       <c r="E219" s="8"/>
@@ -5579,10 +5570,10 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D220" s="8"/>
       <c r="E220" s="8"/>
@@ -5595,10 +5586,10 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D221" s="8"/>
       <c r="E221" s="8"/>
@@ -5611,10 +5602,10 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D222" s="8"/>
       <c r="E222" s="8"/>
@@ -5627,10 +5618,10 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D223" s="8"/>
       <c r="E223" s="8"/>
@@ -5643,10 +5634,10 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D224" s="8"/>
       <c r="E224" s="8"/>
@@ -5659,10 +5650,10 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D225" s="8"/>
       <c r="E225" s="8"/>
@@ -5675,10 +5666,10 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D226" s="8"/>
       <c r="E226" s="8"/>
@@ -5691,10 +5682,10 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D227" s="8"/>
       <c r="E227" s="8"/>
@@ -5707,10 +5698,10 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D228" s="8"/>
       <c r="E228" s="8"/>
@@ -5723,7 +5714,7 @@
     </row>
     <row r="229" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="5" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B229" s="26"/>
       <c r="C229" s="26"/>
@@ -5738,10 +5729,10 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D230" s="8"/>
       <c r="E230" s="8"/>
@@ -5754,10 +5745,10 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D231" s="8"/>
       <c r="E231" s="8"/>
@@ -5770,7 +5761,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="26" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D232" s="8"/>
       <c r="E232" s="8"/>
@@ -5783,10 +5774,10 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D233" s="8"/>
       <c r="E233" s="8"/>
@@ -5799,10 +5790,10 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="8" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D234" s="8"/>
       <c r="E234" s="8"/>
@@ -5815,7 +5806,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="26" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D235" s="8"/>
       <c r="E235" s="8"/>
@@ -5828,10 +5819,10 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="30" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B236" s="30" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D236" s="8"/>
       <c r="E236" s="8"/>
@@ -5844,10 +5835,10 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="30" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B237" s="30" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D237" s="8"/>
       <c r="E237" s="8"/>
@@ -5860,10 +5851,10 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D238" s="8"/>
       <c r="E238" s="8"/>
@@ -5876,10 +5867,10 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D239" s="8"/>
       <c r="E239" s="8"/>
@@ -5892,10 +5883,10 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D240" s="8"/>
       <c r="E240" s="8"/>
@@ -5908,10 +5899,10 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D241" s="8"/>
       <c r="E241" s="8"/>
@@ -5924,10 +5915,10 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D242" s="8"/>
       <c r="E242" s="8"/>
@@ -5940,10 +5931,10 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D243" s="8"/>
       <c r="E243" s="8"/>
@@ -5956,10 +5947,10 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D244" s="8"/>
       <c r="E244" s="8"/>
@@ -5972,7 +5963,7 @@
     </row>
     <row r="245" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="31" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B245" s="31"/>
       <c r="C245" s="31"/>
@@ -5987,10 +5978,10 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D246" s="8"/>
       <c r="E246" s="8"/>
@@ -6003,7 +5994,7 @@
     </row>
     <row r="247" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="31" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B247" s="34"/>
       <c r="C247" s="34"/>
@@ -6016,12 +6007,12 @@
       <c r="J247" s="35"/>
       <c r="K247" s="35"/>
     </row>
-    <row r="248" customFormat="false" ht="57.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="164.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D248" s="8"/>
       <c r="E248" s="8"/>
@@ -6034,7 +6025,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="26" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D249" s="8"/>
       <c r="E249" s="8"/>
@@ -6047,10 +6038,10 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="37" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B250" s="38" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D250" s="8"/>
       <c r="E250" s="8"/>
@@ -6063,10 +6054,10 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="39" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B251" s="40" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D251" s="8"/>
       <c r="E251" s="8"/>
@@ -6079,10 +6070,10 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="41" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B252" s="42" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D252" s="8"/>
       <c r="E252" s="8"/>
@@ -6095,10 +6086,10 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="41" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B253" s="40" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D253" s="8"/>
       <c r="E253" s="8"/>
@@ -6111,10 +6102,10 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="39" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B254" s="40" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D254" s="8"/>
       <c r="E254" s="8"/>
@@ -6127,10 +6118,10 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C255" s="12"/>
       <c r="D255" s="8"/>
@@ -7696,10 +7687,10 @@
     </row>
     <row r="3" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="46" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C3" s="47"/>
       <c r="D3" s="48"/>
@@ -7712,7 +7703,7 @@
     </row>
     <row r="4" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="46" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B4" s="46" t="s">
         <v>8</v>
@@ -7728,10 +7719,10 @@
     </row>
     <row r="5" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="49" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
@@ -7744,10 +7735,10 @@
     </row>
     <row r="6" s="50" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="49" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
@@ -7760,13 +7751,13 @@
     </row>
     <row r="7" s="50" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="49" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D7" s="48"/>
       <c r="E7" s="48"/>
@@ -7778,10 +7769,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -7794,10 +7785,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -7810,10 +7801,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -7826,10 +7817,10 @@
     </row>
     <row r="11" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="49" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C11" s="48"/>
       <c r="D11" s="48"/>
@@ -7842,10 +7833,10 @@
     </row>
     <row r="12" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="49" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C12" s="48"/>
       <c r="D12" s="48"/>
@@ -7858,10 +7849,10 @@
     </row>
     <row r="13" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="49" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C13" s="48"/>
       <c r="D13" s="48"/>
@@ -7892,10 +7883,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -7908,10 +7899,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -7923,10 +7914,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -7938,10 +7929,10 @@
     </row>
     <row r="18" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="49" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C18" s="48"/>
       <c r="D18" s="48"/>
@@ -7954,10 +7945,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="49" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C19" s="48" t="s">
         <v>25</v>
@@ -7972,10 +7963,10 @@
     </row>
     <row r="20" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="49" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
@@ -7987,13 +7978,13 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -8005,13 +7996,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -8023,13 +8014,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -8041,13 +8032,13 @@
     </row>
     <row r="24" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="49" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B24" s="49" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D24" s="48"/>
       <c r="E24" s="48"/>
@@ -8109,13 +8100,13 @@
     </row>
     <row r="30" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -18155,17 +18146,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="76.62"/>
   </cols>
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>25</v>
@@ -18174,7 +18165,7 @@
         <v>20</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -18199,103 +18190,151 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="110.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.3"/>
+  </cols>
   <sheetData>
     <row r="1" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C1" s="28"/>
     </row>
     <row r="2" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C2" s="28"/>
     </row>
     <row r="3" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="51" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C3" s="28"/>
     </row>
     <row r="4" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="51" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C4" s="28"/>
     </row>
     <row r="5" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="51" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C5" s="28"/>
     </row>
     <row r="6" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="51" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C6" s="28"/>
     </row>
     <row r="7" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C7" s="28"/>
     </row>
     <row r="8" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="51" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C8" s="28"/>
     </row>
     <row r="9" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="51" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C9" s="28"/>
     </row>
     <row r="10" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="51" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C10" s="28"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="E13" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Updated linting rules to clean up ORIQ -- this update was done months ago but changes had been lost somehow
</commit_message>
<xml_diff>
--- a/config_new.xlsx
+++ b/config_new.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="490">
   <si>
     <t xml:space="preserve">search</t>
   </si>
@@ -1824,6 +1824,46 @@
     <t xml:space="preserve">&lt;em&gt;‌‘$1’</t>
   </si>
   <si>
+    <t xml:space="preserve">### xyz ###</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;span class="txt-underline"&gt;(To answer:|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">To change your answer:|Practice)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(\s*&lt;/span&gt;\s*)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;span class="txt-underline"&gt;‌$1‌&lt;/span&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;For this type of question you will type your answer in a box.&lt;br/&gt;Practise typing in the box below.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;‌For this type of question you will type your answer in a box.&lt;br/&gt;Practise typing in the box below.‌&lt;/strong&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">'fragments'</t>
   </si>
   <si>
@@ -2041,7 +2081,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2182,6 +2222,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2468,7 +2513,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2582,9 +2627,9 @@
   <dimension ref="A1:AN1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A243" activeCellId="0" sqref="A243"/>
+      <selection pane="bottomLeft" activeCell="A264" activeCellId="0" sqref="A264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6134,6 +6179,9 @@
       <c r="K255" s="8"/>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="31" t="s">
+        <v>428</v>
+      </c>
       <c r="D256" s="8"/>
       <c r="E256" s="8"/>
       <c r="F256" s="8"/>
@@ -6144,6 +6192,12 @@
       <c r="K256" s="8"/>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="D257" s="8"/>
       <c r="E257" s="8"/>
       <c r="F257" s="8"/>
@@ -6154,6 +6208,12 @@
       <c r="K257" s="8"/>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>432</v>
+      </c>
       <c r="D258" s="8"/>
       <c r="E258" s="8"/>
       <c r="F258" s="8"/>
@@ -7687,10 +7747,10 @@
     </row>
     <row r="3" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="46" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="C3" s="47"/>
       <c r="D3" s="48"/>
@@ -7703,7 +7763,7 @@
     </row>
     <row r="4" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="46" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="B4" s="46" t="s">
         <v>8</v>
@@ -7719,7 +7779,7 @@
     </row>
     <row r="5" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="49" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="B5" s="49" t="s">
         <v>201</v>
@@ -7735,10 +7795,10 @@
     </row>
     <row r="6" s="50" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="49" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
@@ -7769,7 +7829,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>53</v>
@@ -7785,7 +7845,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>53</v>
@@ -7801,10 +7861,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -7817,10 +7877,10 @@
     </row>
     <row r="11" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="49" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="C11" s="48"/>
       <c r="D11" s="48"/>
@@ -7833,10 +7893,10 @@
     </row>
     <row r="12" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="49" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="C12" s="48"/>
       <c r="D12" s="48"/>
@@ -7849,10 +7909,10 @@
     </row>
     <row r="13" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="49" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="C13" s="48"/>
       <c r="D13" s="48"/>
@@ -7883,7 +7943,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>214</v>
@@ -7899,7 +7959,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>81</v>
@@ -7914,7 +7974,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>81</v>
@@ -7963,7 +8023,7 @@
     </row>
     <row r="20" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="49" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="C20" s="48" t="s">
         <v>81</v>
@@ -7984,7 +8044,7 @@
         <v>145</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -8002,7 +8062,7 @@
         <v>148</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -8014,13 +8074,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -8032,13 +8092,13 @@
     </row>
     <row r="24" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="49" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="B24" s="49" t="s">
         <v>234</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="D24" s="48"/>
       <c r="E24" s="48"/>
@@ -8100,13 +8160,13 @@
     </row>
     <row r="30" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -18146,17 +18206,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="76.62"/>
   </cols>
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>25</v>
@@ -18165,7 +18225,7 @@
         <v>20</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -18193,10 +18253,10 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="110.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.52"/>
@@ -18205,91 +18265,91 @@
   <sheetData>
     <row r="1" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="C1" s="28"/>
     </row>
     <row r="2" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="C2" s="28"/>
     </row>
     <row r="3" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="51" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="C3" s="28"/>
     </row>
     <row r="4" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="51" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="C4" s="28"/>
     </row>
     <row r="5" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="51" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="C5" s="28"/>
     </row>
     <row r="6" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="51" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="C6" s="28"/>
     </row>
     <row r="7" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="C7" s="28"/>
     </row>
     <row r="8" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="51" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="C8" s="28"/>
     </row>
     <row r="9" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="51" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="C9" s="28"/>
     </row>
     <row r="10" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="51" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="C10" s="28"/>
     </row>
@@ -18301,10 +18361,10 @@
         <v>169</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18315,24 +18375,24 @@
         <v>44</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="E13" s="13"/>
     </row>

</xml_diff>

<commit_message>
Updated regex to match only spaces in XYZ and not LF
</commit_message>
<xml_diff>
--- a/config_new.xlsx
+++ b/config_new.xlsx
@@ -1827,32 +1827,7 @@
     <t xml:space="preserve">### xyz ###</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;span class="txt-underline"&gt;(To answer:|</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">To change your answer:|Practice)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(\s*&lt;/span&gt;\s*)</t>
-    </r>
+    <t xml:space="preserve">&lt;span class="txt-underline"&gt;(To answer:|To change your answer:|Practice)([ ]*&lt;/span&gt;[ ]*)</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;span class="txt-underline"&gt;‌$1‌&lt;/span&gt; </t>
@@ -2081,7 +2056,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2222,11 +2197,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2513,7 +2483,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2627,9 +2597,9 @@
   <dimension ref="A1:AN1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A264" activeCellId="0" sqref="A264"/>
+      <selection pane="bottomLeft" activeCell="A248" activeCellId="0" sqref="A248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18206,7 +18176,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="76.62"/>
   </cols>
@@ -18256,7 +18226,7 @@
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="110.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.52"/>

</xml_diff>